<commit_message>
ADD: Results from evaluating different prompts
</commit_message>
<xml_diff>
--- a/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
+++ b/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>promptCOT01</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.338</v>
+        <v>0.477</v>
       </c>
       <c r="E2" t="n">
-        <v>0.333</v>
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.275</v>
+        <v>0.496</v>
       </c>
       <c r="G2" t="n">
-        <v>0.333</v>
+        <v>0.5</v>
       </c>
       <c r="H2" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.063</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
@@ -553,12 +553,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -567,33 +567,33 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.622</v>
+        <v>0.652</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.707</v>
       </c>
       <c r="F4" t="n">
-        <v>0.661</v>
+        <v>0.699</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.707</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -602,33 +602,33 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.632</v>
+        <v>0.622</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.661</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -637,33 +637,33 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.454</v>
+        <v>0.632</v>
       </c>
       <c r="E6" t="n">
-        <v>0.52</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>0.507</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>0.52</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.516</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -672,33 +672,33 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.582</v>
+        <v>0.601</v>
       </c>
       <c r="E7" t="n">
-        <v>0.637</v>
+        <v>0.667</v>
       </c>
       <c r="F7" t="n">
-        <v>0.626</v>
+        <v>0.636</v>
       </c>
       <c r="G7" t="n">
-        <v>0.637</v>
+        <v>0.667</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.627</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,33 +707,33 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.608</v>
+        <v>0.6</v>
       </c>
       <c r="E8" t="n">
-        <v>0.667</v>
+        <v>0.65</v>
       </c>
       <c r="F8" t="n">
-        <v>0.643</v>
+        <v>0.642</v>
       </c>
       <c r="G8" t="n">
-        <v>0.667</v>
+        <v>0.65</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" t="n">
-        <v>0.667</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -742,22 +742,22 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.582</v>
+        <v>0.454</v>
       </c>
       <c r="E9" t="n">
-        <v>0.639</v>
+        <v>0.52</v>
       </c>
       <c r="F9" t="n">
-        <v>0.621</v>
+        <v>0.507</v>
       </c>
       <c r="G9" t="n">
-        <v>0.639</v>
+        <v>0.52</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.619</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="10">
@@ -768,7 +768,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -777,28 +777,28 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.654</v>
+        <v>0.647</v>
       </c>
       <c r="E10" t="n">
-        <v>0.696</v>
+        <v>0.694</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.696</v>
+        <v>0.694</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -812,33 +812,33 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.639</v>
+        <v>0.597</v>
       </c>
       <c r="E11" t="n">
-        <v>0.68</v>
+        <v>0.659</v>
       </c>
       <c r="F11" t="n">
-        <v>0.67</v>
+        <v>0.632</v>
       </c>
       <c r="G11" t="n">
-        <v>0.68</v>
+        <v>0.659</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>0.675</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -847,33 +847,33 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.594</v>
+        <v>0.582</v>
       </c>
       <c r="E12" t="n">
-        <v>0.656</v>
+        <v>0.637</v>
       </c>
       <c r="F12" t="n">
-        <v>0.631</v>
+        <v>0.626</v>
       </c>
       <c r="G12" t="n">
-        <v>0.656</v>
+        <v>0.637</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>0.651</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -882,33 +882,33 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.597</v>
+        <v>0.652</v>
       </c>
       <c r="E13" t="n">
-        <v>0.643</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>0.637</v>
+        <v>0.681</v>
       </c>
       <c r="G13" t="n">
-        <v>0.643</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.643</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>promptCOT02</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -917,33 +917,33 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.496</v>
+        <v>0.608</v>
       </c>
       <c r="E14" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
       </c>
       <c r="F14" t="n">
-        <v>0.535</v>
+        <v>0.643</v>
       </c>
       <c r="G14" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -952,19 +952,19 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.571</v>
+        <v>0.582</v>
       </c>
       <c r="E15" t="n">
-        <v>0.619</v>
+        <v>0.639</v>
       </c>
       <c r="F15" t="n">
-        <v>0.613</v>
+        <v>0.621</v>
       </c>
       <c r="G15" t="n">
-        <v>0.619</v>
+        <v>0.639</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
         <v>0.619</v>
@@ -973,12 +973,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>promptCOT01</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -987,33 +987,33 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.497</v>
+        <v>0.654</v>
       </c>
       <c r="E16" t="n">
-        <v>0.516</v>
+        <v>0.696</v>
       </c>
       <c r="F16" t="n">
-        <v>0.522</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="G16" t="n">
-        <v>0.516</v>
+        <v>0.696</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>0.516</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1022,33 +1022,33 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.668</v>
+        <v>0.639</v>
       </c>
       <c r="E17" t="n">
-        <v>0.717</v>
+        <v>0.68</v>
       </c>
       <c r="F17" t="n">
-        <v>0.714</v>
+        <v>0.67</v>
       </c>
       <c r="G17" t="n">
-        <v>0.717</v>
+        <v>0.68</v>
       </c>
       <c r="H17" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1057,33 +1057,33 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.614</v>
+        <v>0.594</v>
       </c>
       <c r="E18" t="n">
-        <v>0.675</v>
+        <v>0.656</v>
       </c>
       <c r="F18" t="n">
-        <v>0.664</v>
+        <v>0.631</v>
       </c>
       <c r="G18" t="n">
-        <v>0.675</v>
+        <v>0.656</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>0.675</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1092,33 +1092,33 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.508</v>
+        <v>0.57</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.635</v>
       </c>
       <c r="F19" t="n">
-        <v>0.555</v>
+        <v>0.623</v>
       </c>
       <c r="G19" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.635</v>
       </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.556</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1127,22 +1127,22 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.531</v>
+        <v>0.597</v>
       </c>
       <c r="E20" t="n">
-        <v>0.603</v>
+        <v>0.643</v>
       </c>
       <c r="F20" t="n">
-        <v>0.588</v>
+        <v>0.637</v>
       </c>
       <c r="G20" t="n">
-        <v>0.603</v>
+        <v>0.643</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0.603</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="21">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1162,33 +1162,33 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.648</v>
+        <v>0.656</v>
       </c>
       <c r="E21" t="n">
-        <v>0.694</v>
+        <v>0.696</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>0.694</v>
+        <v>0.696</v>
       </c>
       <c r="H21" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>0.667</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1197,33 +1197,33 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.611</v>
+        <v>0.571</v>
       </c>
       <c r="E22" t="n">
-        <v>0.675</v>
+        <v>0.619</v>
       </c>
       <c r="F22" t="n">
-        <v>0.647</v>
+        <v>0.613</v>
       </c>
       <c r="G22" t="n">
-        <v>0.675</v>
+        <v>0.619</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0.675</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>promptCOT01</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1232,33 +1232,33 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.524</v>
+        <v>0.668</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.717</v>
       </c>
       <c r="F23" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.714</v>
       </c>
       <c r="G23" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.717</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I23" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>promptCOT02</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1267,33 +1267,33 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.477</v>
+        <v>0.51</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="F24" t="n">
-        <v>0.496</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0.5</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1302,33 +1302,33 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.481</v>
+        <v>0.614</v>
       </c>
       <c r="E25" t="n">
-        <v>0.524</v>
+        <v>0.675</v>
       </c>
       <c r="F25" t="n">
-        <v>0.529</v>
+        <v>0.664</v>
       </c>
       <c r="G25" t="n">
-        <v>0.524</v>
+        <v>0.675</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.524</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1337,33 +1337,33 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.508</v>
       </c>
       <c r="E26" t="n">
-        <v>0.724</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F26" t="n">
-        <v>0.72</v>
+        <v>0.555</v>
       </c>
       <c r="G26" t="n">
-        <v>0.724</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>0.706</v>
+        <v>0.556</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1372,28 +1372,28 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.607</v>
+        <v>0.497</v>
       </c>
       <c r="E27" t="n">
-        <v>0.656</v>
+        <v>0.516</v>
       </c>
       <c r="F27" t="n">
-        <v>0.627</v>
+        <v>0.522</v>
       </c>
       <c r="G27" t="n">
-        <v>0.656</v>
+        <v>0.516</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>0.651</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1407,33 +1407,33 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.574</v>
+        <v>0.531</v>
       </c>
       <c r="E28" t="n">
-        <v>0.627</v>
+        <v>0.603</v>
       </c>
       <c r="F28" t="n">
-        <v>0.628</v>
+        <v>0.588</v>
       </c>
       <c r="G28" t="n">
-        <v>0.627</v>
+        <v>0.603</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>0.627</v>
+        <v>0.603</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1442,33 +1442,33 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.645</v>
+        <v>0.615</v>
       </c>
       <c r="E29" t="n">
-        <v>0.68</v>
+        <v>0.651</v>
       </c>
       <c r="F29" t="n">
-        <v>0.67</v>
+        <v>0.647</v>
       </c>
       <c r="G29" t="n">
-        <v>0.68</v>
+        <v>0.651</v>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>0.675</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1477,33 +1477,33 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.609</v>
+        <v>0.648</v>
       </c>
       <c r="E30" t="n">
-        <v>0.669</v>
+        <v>0.694</v>
       </c>
       <c r="F30" t="n">
-        <v>0.644</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G30" t="n">
-        <v>0.669</v>
+        <v>0.694</v>
       </c>
       <c r="H30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I30" t="n">
-        <v>0.659</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>promptCOT02</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1512,33 +1512,33 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.516</v>
+        <v>0.608</v>
       </c>
       <c r="E31" t="n">
-        <v>0.571</v>
+        <v>0.659</v>
       </c>
       <c r="F31" t="n">
-        <v>0.569</v>
+        <v>0.645</v>
       </c>
       <c r="G31" t="n">
-        <v>0.571</v>
+        <v>0.659</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>0.571</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1547,33 +1547,33 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.617</v>
+        <v>0.496</v>
       </c>
       <c r="E32" t="n">
-        <v>0.664</v>
+        <v>0.524</v>
       </c>
       <c r="F32" t="n">
-        <v>0.651</v>
+        <v>0.535</v>
       </c>
       <c r="G32" t="n">
-        <v>0.664</v>
+        <v>0.524</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>0.659</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1582,19 +1582,19 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.597</v>
+        <v>0.607</v>
       </c>
       <c r="E33" t="n">
-        <v>0.659</v>
+        <v>0.664</v>
       </c>
       <c r="F33" t="n">
-        <v>0.64</v>
+        <v>0.644</v>
       </c>
       <c r="G33" t="n">
-        <v>0.659</v>
+        <v>0.664</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
         <v>0.659</v>
@@ -1603,12 +1603,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1617,33 +1617,33 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.414</v>
+        <v>0.516</v>
       </c>
       <c r="E34" t="n">
-        <v>0.472</v>
+        <v>0.571</v>
       </c>
       <c r="F34" t="n">
-        <v>0.46</v>
+        <v>0.569</v>
       </c>
       <c r="G34" t="n">
-        <v>0.472</v>
+        <v>0.571</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0.468</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1652,33 +1652,33 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.614</v>
+        <v>0.611</v>
       </c>
       <c r="E35" t="n">
-        <v>0.664</v>
+        <v>0.675</v>
       </c>
       <c r="F35" t="n">
-        <v>0.648</v>
+        <v>0.647</v>
       </c>
       <c r="G35" t="n">
-        <v>0.664</v>
+        <v>0.675</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>0.659</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1687,33 +1687,33 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.536</v>
+        <v>0.619</v>
       </c>
       <c r="E36" t="n">
-        <v>0.576</v>
+        <v>0.675</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.662</v>
       </c>
       <c r="G36" t="n">
-        <v>0.576</v>
+        <v>0.675</v>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.571</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1722,56 +1722,721 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.587</v>
+        <v>0.596</v>
       </c>
       <c r="E37" t="n">
-        <v>0.643</v>
+        <v>0.656</v>
       </c>
       <c r="F37" t="n">
-        <v>0.626</v>
+        <v>0.652</v>
       </c>
       <c r="G37" t="n">
-        <v>0.643</v>
+        <v>0.656</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>0.643</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.651</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H39" t="n">
+        <v>102</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.063</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.595</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>promptN06</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.481</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.529</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.524</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>promptN05</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.6919999999999999</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.706</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.607</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.651</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.628</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>promptN08</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.675</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>promptN09</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.651</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.6909999999999999</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.698</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>promptN04</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.597</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>promptN09</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.667</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.414</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.468</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>promptN06</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.614</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.648</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>promptN09</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.536</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.571</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>promptN07</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.621</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.651</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>promptN03</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.643</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>promptN01</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>gemini-1.5-pro</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>level1</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
         <v>0.59</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E57" t="n">
         <v>0.651</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F57" t="n">
         <v>0.648</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G57" t="n">
         <v>0.651</v>
       </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
         <v>0.651</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add: include GPT-based discourse relation parsing results and apply minor unrelated modifications
</commit_message>
<xml_diff>
--- a/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
+++ b/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,12 +553,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -567,33 +567,33 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.652</v>
+        <v>0.435</v>
       </c>
       <c r="E4" t="n">
-        <v>0.707</v>
+        <v>0.484</v>
       </c>
       <c r="F4" t="n">
-        <v>0.699</v>
+        <v>0.491</v>
       </c>
       <c r="G4" t="n">
-        <v>0.707</v>
+        <v>0.484</v>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.484</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -602,33 +602,33 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.622</v>
+        <v>0.652</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.707</v>
       </c>
       <c r="F5" t="n">
-        <v>0.661</v>
+        <v>0.699</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.707</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -637,33 +637,33 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.632</v>
+        <v>0.622</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.661</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.601</v>
+        <v>0.632</v>
       </c>
       <c r="E7" t="n">
-        <v>0.667</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>0.636</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G7" t="n">
-        <v>0.667</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.667</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -698,7 +698,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,33 +707,33 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.6</v>
+        <v>0.548</v>
       </c>
       <c r="E8" t="n">
-        <v>0.65</v>
+        <v>0.587</v>
       </c>
       <c r="F8" t="n">
-        <v>0.642</v>
+        <v>0.582</v>
       </c>
       <c r="G8" t="n">
-        <v>0.65</v>
+        <v>0.587</v>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.635</v>
+        <v>0.587</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -742,28 +742,28 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.454</v>
+        <v>0.601</v>
       </c>
       <c r="E9" t="n">
-        <v>0.52</v>
+        <v>0.667</v>
       </c>
       <c r="F9" t="n">
-        <v>0.507</v>
+        <v>0.636</v>
       </c>
       <c r="G9" t="n">
-        <v>0.52</v>
+        <v>0.667</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.516</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,33 +777,33 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.647</v>
+        <v>0.6</v>
       </c>
       <c r="E10" t="n">
-        <v>0.694</v>
+        <v>0.65</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.642</v>
       </c>
       <c r="G10" t="n">
-        <v>0.694</v>
+        <v>0.65</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -812,28 +812,28 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.597</v>
+        <v>0.454</v>
       </c>
       <c r="E11" t="n">
-        <v>0.659</v>
+        <v>0.52</v>
       </c>
       <c r="F11" t="n">
-        <v>0.632</v>
+        <v>0.507</v>
       </c>
       <c r="G11" t="n">
-        <v>0.659</v>
+        <v>0.52</v>
       </c>
       <c r="H11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.643</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -847,33 +847,33 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.582</v>
+        <v>0.647</v>
       </c>
       <c r="E12" t="n">
-        <v>0.637</v>
+        <v>0.694</v>
       </c>
       <c r="F12" t="n">
-        <v>0.626</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="G12" t="n">
-        <v>0.637</v>
+        <v>0.694</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>0.627</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -882,28 +882,28 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.652</v>
+        <v>0.486</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.524</v>
       </c>
       <c r="F13" t="n">
-        <v>0.681</v>
+        <v>0.529</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.524</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -917,28 +917,28 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.608</v>
+        <v>0.597</v>
       </c>
       <c r="E14" t="n">
-        <v>0.667</v>
+        <v>0.659</v>
       </c>
       <c r="F14" t="n">
+        <v>0.632</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.643</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.667</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.667</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -955,30 +955,30 @@
         <v>0.582</v>
       </c>
       <c r="E15" t="n">
-        <v>0.639</v>
+        <v>0.637</v>
       </c>
       <c r="F15" t="n">
-        <v>0.621</v>
+        <v>0.626</v>
       </c>
       <c r="G15" t="n">
-        <v>0.639</v>
+        <v>0.637</v>
       </c>
       <c r="H15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I15" t="n">
-        <v>0.619</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -987,33 +987,33 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.654</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>0.696</v>
+        <v>0.726</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.722</v>
       </c>
       <c r="G16" t="n">
-        <v>0.696</v>
+        <v>0.726</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.714</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1022,33 +1022,33 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.639</v>
+        <v>0.598</v>
       </c>
       <c r="E17" t="n">
-        <v>0.68</v>
+        <v>0.659</v>
       </c>
       <c r="F17" t="n">
-        <v>0.67</v>
+        <v>0.64</v>
       </c>
       <c r="G17" t="n">
-        <v>0.68</v>
+        <v>0.659</v>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.675</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1057,33 +1057,33 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.594</v>
+        <v>0.587</v>
       </c>
       <c r="E18" t="n">
-        <v>0.656</v>
+        <v>0.633</v>
       </c>
       <c r="F18" t="n">
-        <v>0.631</v>
+        <v>0.622</v>
       </c>
       <c r="G18" t="n">
-        <v>0.656</v>
+        <v>0.633</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I18" t="n">
-        <v>0.651</v>
+        <v>0.603</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1092,33 +1092,33 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.57</v>
+        <v>0.652</v>
       </c>
       <c r="E19" t="n">
-        <v>0.635</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>0.623</v>
+        <v>0.681</v>
       </c>
       <c r="G19" t="n">
-        <v>0.635</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.635</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1127,33 +1127,33 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.597</v>
+        <v>0.608</v>
       </c>
       <c r="E20" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="F20" t="n">
         <v>0.643</v>
       </c>
-      <c r="F20" t="n">
-        <v>0.637</v>
-      </c>
       <c r="G20" t="n">
-        <v>0.643</v>
+        <v>0.667</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0.643</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1162,33 +1162,33 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.656</v>
+        <v>0.582</v>
       </c>
       <c r="E21" t="n">
-        <v>0.696</v>
+        <v>0.639</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.621</v>
       </c>
       <c r="G21" t="n">
-        <v>0.696</v>
+        <v>0.639</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I21" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1197,33 +1197,33 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.571</v>
+        <v>0.654</v>
       </c>
       <c r="E22" t="n">
-        <v>0.619</v>
+        <v>0.696</v>
       </c>
       <c r="F22" t="n">
-        <v>0.613</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="G22" t="n">
-        <v>0.619</v>
+        <v>0.696</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>0.619</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1232,28 +1232,28 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.668</v>
+        <v>0.639</v>
       </c>
       <c r="E23" t="n">
-        <v>0.717</v>
+        <v>0.68</v>
       </c>
       <c r="F23" t="n">
-        <v>0.714</v>
+        <v>0.67</v>
       </c>
       <c r="G23" t="n">
-        <v>0.717</v>
+        <v>0.68</v>
       </c>
       <c r="H23" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1267,22 +1267,22 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.51</v>
+        <v>0.594</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.656</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.631</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.656</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="25">
@@ -1302,33 +1302,33 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.614</v>
+        <v>0.57</v>
       </c>
       <c r="E25" t="n">
-        <v>0.675</v>
+        <v>0.635</v>
       </c>
       <c r="F25" t="n">
-        <v>0.664</v>
+        <v>0.623</v>
       </c>
       <c r="G25" t="n">
-        <v>0.675</v>
+        <v>0.635</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.675</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1337,33 +1337,33 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.508</v>
+        <v>0.597</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.643</v>
       </c>
       <c r="F26" t="n">
-        <v>0.555</v>
+        <v>0.637</v>
       </c>
       <c r="G26" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.643</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>0.556</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1372,33 +1372,33 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.497</v>
+        <v>0.536</v>
       </c>
       <c r="E27" t="n">
-        <v>0.516</v>
+        <v>0.571</v>
       </c>
       <c r="F27" t="n">
-        <v>0.522</v>
+        <v>0.554</v>
       </c>
       <c r="G27" t="n">
-        <v>0.516</v>
+        <v>0.571</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>0.516</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1407,28 +1407,28 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.531</v>
+        <v>0.656</v>
       </c>
       <c r="E28" t="n">
-        <v>0.603</v>
+        <v>0.696</v>
       </c>
       <c r="F28" t="n">
-        <v>0.588</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G28" t="n">
-        <v>0.603</v>
+        <v>0.696</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
-        <v>0.603</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1442,33 +1442,33 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.615</v>
+        <v>0.508</v>
       </c>
       <c r="E29" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
       </c>
       <c r="F29" t="n">
-        <v>0.647</v>
+        <v>0.538</v>
       </c>
       <c r="G29" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1477,28 +1477,28 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.648</v>
+        <v>0.571</v>
       </c>
       <c r="E30" t="n">
-        <v>0.694</v>
+        <v>0.619</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.613</v>
       </c>
       <c r="G30" t="n">
-        <v>0.694</v>
+        <v>0.619</v>
       </c>
       <c r="H30" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0.667</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1512,22 +1512,22 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.608</v>
+        <v>0.668</v>
       </c>
       <c r="E31" t="n">
-        <v>0.659</v>
+        <v>0.717</v>
       </c>
       <c r="F31" t="n">
-        <v>0.645</v>
+        <v>0.714</v>
       </c>
       <c r="G31" t="n">
-        <v>0.659</v>
+        <v>0.717</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I31" t="n">
-        <v>0.659</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1547,33 +1547,33 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.496</v>
+        <v>0.51</v>
       </c>
       <c r="E32" t="n">
-        <v>0.524</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="F32" t="n">
-        <v>0.535</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="G32" t="n">
-        <v>0.524</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>0.524</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1582,33 +1582,33 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.607</v>
+        <v>0.614</v>
       </c>
       <c r="E33" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="F33" t="n">
         <v>0.664</v>
       </c>
-      <c r="F33" t="n">
-        <v>0.644</v>
-      </c>
       <c r="G33" t="n">
-        <v>0.664</v>
+        <v>0.675</v>
       </c>
       <c r="H33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>0.659</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1617,13 +1617,13 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.516</v>
+        <v>0.509</v>
       </c>
       <c r="E34" t="n">
         <v>0.571</v>
       </c>
       <c r="F34" t="n">
-        <v>0.569</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G34" t="n">
         <v>0.571</v>
@@ -1638,12 +1638,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1652,33 +1652,33 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.611</v>
+        <v>0.508</v>
       </c>
       <c r="E35" t="n">
-        <v>0.675</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F35" t="n">
-        <v>0.647</v>
+        <v>0.555</v>
       </c>
       <c r="G35" t="n">
-        <v>0.675</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0.675</v>
+        <v>0.556</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1687,33 +1687,33 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.619</v>
+        <v>0.506</v>
       </c>
       <c r="E36" t="n">
-        <v>0.675</v>
+        <v>0.552</v>
       </c>
       <c r="F36" t="n">
-        <v>0.662</v>
+        <v>0.55</v>
       </c>
       <c r="G36" t="n">
-        <v>0.675</v>
+        <v>0.552</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>0.675</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1722,33 +1722,33 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.596</v>
+        <v>0.497</v>
       </c>
       <c r="E37" t="n">
-        <v>0.656</v>
+        <v>0.516</v>
       </c>
       <c r="F37" t="n">
-        <v>0.652</v>
+        <v>0.522</v>
       </c>
       <c r="G37" t="n">
-        <v>0.656</v>
+        <v>0.516</v>
       </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0.651</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1757,28 +1757,28 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.605</v>
+        <v>0.471</v>
       </c>
       <c r="E38" t="n">
-        <v>0.656</v>
+        <v>0.532</v>
       </c>
       <c r="F38" t="n">
-        <v>0.643</v>
+        <v>0.502</v>
       </c>
       <c r="G38" t="n">
-        <v>0.656</v>
+        <v>0.532</v>
       </c>
       <c r="H38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1792,33 +1792,33 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.338</v>
+        <v>0.531</v>
       </c>
       <c r="E39" t="n">
-        <v>0.333</v>
+        <v>0.603</v>
       </c>
       <c r="F39" t="n">
-        <v>0.275</v>
+        <v>0.588</v>
       </c>
       <c r="G39" t="n">
-        <v>0.333</v>
+        <v>0.603</v>
       </c>
       <c r="H39" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0.063</v>
+        <v>0.603</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1827,33 +1827,33 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.549</v>
+        <v>0.615</v>
       </c>
       <c r="E40" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
       </c>
       <c r="F40" t="n">
-        <v>0.587</v>
+        <v>0.647</v>
       </c>
       <c r="G40" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1862,33 +1862,33 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.481</v>
+        <v>0.648</v>
       </c>
       <c r="E41" t="n">
-        <v>0.524</v>
+        <v>0.694</v>
       </c>
       <c r="F41" t="n">
-        <v>0.529</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G41" t="n">
-        <v>0.524</v>
+        <v>0.694</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I41" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1897,33 +1897,33 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.548</v>
       </c>
       <c r="E42" t="n">
-        <v>0.724</v>
+        <v>0.595</v>
       </c>
       <c r="F42" t="n">
-        <v>0.72</v>
+        <v>0.586</v>
       </c>
       <c r="G42" t="n">
-        <v>0.724</v>
+        <v>0.595</v>
       </c>
       <c r="H42" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0.706</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1932,33 +1932,33 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.607</v>
+        <v>0.608</v>
       </c>
       <c r="E43" t="n">
-        <v>0.656</v>
+        <v>0.659</v>
       </c>
       <c r="F43" t="n">
-        <v>0.627</v>
+        <v>0.645</v>
       </c>
       <c r="G43" t="n">
-        <v>0.656</v>
+        <v>0.659</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>0.651</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1967,28 +1967,28 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.574</v>
+        <v>0.496</v>
       </c>
       <c r="E44" t="n">
-        <v>0.627</v>
+        <v>0.524</v>
       </c>
       <c r="F44" t="n">
-        <v>0.628</v>
+        <v>0.535</v>
       </c>
       <c r="G44" t="n">
-        <v>0.627</v>
+        <v>0.524</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>0.627</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2002,28 +2002,28 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.645</v>
+        <v>0.607</v>
       </c>
       <c r="E45" t="n">
-        <v>0.68</v>
+        <v>0.664</v>
       </c>
       <c r="F45" t="n">
-        <v>0.67</v>
+        <v>0.644</v>
       </c>
       <c r="G45" t="n">
-        <v>0.68</v>
+        <v>0.664</v>
       </c>
       <c r="H45" t="n">
         <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>0.675</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2037,33 +2037,33 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.609</v>
+        <v>0.516</v>
       </c>
       <c r="E46" t="n">
-        <v>0.669</v>
+        <v>0.571</v>
       </c>
       <c r="F46" t="n">
-        <v>0.644</v>
+        <v>0.569</v>
       </c>
       <c r="G46" t="n">
-        <v>0.669</v>
+        <v>0.571</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2072,33 +2072,33 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.617</v>
+        <v>0.524</v>
       </c>
       <c r="E47" t="n">
-        <v>0.664</v>
+        <v>0.548</v>
       </c>
       <c r="F47" t="n">
-        <v>0.651</v>
+        <v>0.553</v>
       </c>
       <c r="G47" t="n">
-        <v>0.664</v>
+        <v>0.548</v>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>0.659</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2107,33 +2107,33 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.644</v>
+        <v>0.611</v>
       </c>
       <c r="E48" t="n">
-        <v>0.698</v>
+        <v>0.675</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.647</v>
       </c>
       <c r="G48" t="n">
-        <v>0.698</v>
+        <v>0.675</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>0.698</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2142,28 +2142,28 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.597</v>
+        <v>0.619</v>
       </c>
       <c r="E49" t="n">
-        <v>0.659</v>
+        <v>0.675</v>
       </c>
       <c r="F49" t="n">
-        <v>0.64</v>
+        <v>0.662</v>
       </c>
       <c r="G49" t="n">
-        <v>0.659</v>
+        <v>0.675</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>0.659</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2177,28 +2177,28 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.626</v>
+        <v>0.596</v>
       </c>
       <c r="E50" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.656</v>
       </c>
       <c r="F50" t="n">
-        <v>0.663</v>
+        <v>0.652</v>
       </c>
       <c r="G50" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.656</v>
       </c>
       <c r="H50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>0.667</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2212,28 +2212,28 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.524</v>
+        <v>0.605</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.656</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.643</v>
       </c>
       <c r="G51" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.656</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2247,33 +2247,33 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.414</v>
+        <v>0.338</v>
       </c>
       <c r="E52" t="n">
-        <v>0.472</v>
+        <v>0.333</v>
       </c>
       <c r="F52" t="n">
-        <v>0.46</v>
+        <v>0.275</v>
       </c>
       <c r="G52" t="n">
-        <v>0.472</v>
+        <v>0.333</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="I52" t="n">
-        <v>0.468</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2282,33 +2282,33 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.614</v>
+        <v>0.341</v>
       </c>
       <c r="E53" t="n">
-        <v>0.664</v>
+        <v>0.413</v>
       </c>
       <c r="F53" t="n">
-        <v>0.648</v>
+        <v>0.401</v>
       </c>
       <c r="G53" t="n">
-        <v>0.664</v>
+        <v>0.413</v>
       </c>
       <c r="H53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>0.659</v>
+        <v>0.413</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2317,33 +2317,33 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.536</v>
+        <v>0.549</v>
       </c>
       <c r="E54" t="n">
-        <v>0.576</v>
+        <v>0.595</v>
       </c>
       <c r="F54" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.587</v>
       </c>
       <c r="G54" t="n">
-        <v>0.576</v>
+        <v>0.595</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
-        <v>0.571</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2352,28 +2352,28 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.621</v>
+        <v>0.481</v>
       </c>
       <c r="E55" t="n">
-        <v>0.667</v>
+        <v>0.524</v>
       </c>
       <c r="F55" t="n">
-        <v>0.659</v>
+        <v>0.529</v>
       </c>
       <c r="G55" t="n">
-        <v>0.667</v>
+        <v>0.524</v>
       </c>
       <c r="H55" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I55" t="n">
-        <v>0.651</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2387,56 +2387,616 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.587</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="E56" t="n">
-        <v>0.643</v>
+        <v>0.724</v>
       </c>
       <c r="F56" t="n">
-        <v>0.626</v>
+        <v>0.72</v>
       </c>
       <c r="G56" t="n">
-        <v>0.643</v>
+        <v>0.724</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I56" t="n">
-        <v>0.643</v>
+        <v>0.706</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.607</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.651</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.628</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>promptN08</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.675</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.317</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="H60" t="n">
+        <v>100</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.079</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>promptN09</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="H61" t="n">
+        <v>2</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.651</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>promptN02</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.6909999999999999</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.698</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>promptN04</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.597</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>promptN09</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="H65" t="n">
+        <v>3</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.667</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>promptN01</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.675</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>promptN10</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.414</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="H68" t="n">
+        <v>1</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.468</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>promptN06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.614</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.648</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="H69" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.659</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>promptN09</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.536</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="H70" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.571</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>promptN07</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.621</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="H71" t="n">
+        <v>3</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.651</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>promptN03</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.643</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>promptN01</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>gemini-1.5-pro</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>level1</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
         <v>0.59</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E73" t="n">
         <v>0.651</v>
       </c>
-      <c r="F57" t="n">
+      <c r="F73" t="n">
         <v>0.648</v>
       </c>
-      <c r="G57" t="n">
+      <c r="G73" t="n">
         <v>0.651</v>
       </c>
-      <c r="H57" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" t="n">
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
         <v>0.651</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chore: Rename result json files to distinguish trial 1 (_t1) and trial 2 (_t2)
</commit_message>
<xml_diff>
--- a/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
+++ b/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -497,33 +497,33 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.477</v>
+        <v>0.6</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="F2" t="n">
-        <v>0.496</v>
+        <v>0.642</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,33 +532,33 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.644</v>
       </c>
       <c r="E3" t="n">
-        <v>0.603</v>
+        <v>0.698</v>
       </c>
       <c r="F3" t="n">
-        <v>0.595</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>0.603</v>
+        <v>0.698</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.603</v>
+        <v>0.698</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -567,33 +567,33 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.435</v>
+        <v>0.652</v>
       </c>
       <c r="E4" t="n">
-        <v>0.484</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0.491</v>
+        <v>0.681</v>
       </c>
       <c r="G4" t="n">
-        <v>0.484</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.484</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -602,33 +602,33 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.652</v>
+        <v>0.516</v>
       </c>
       <c r="E5" t="n">
-        <v>0.707</v>
+        <v>0.571</v>
       </c>
       <c r="F5" t="n">
-        <v>0.699</v>
+        <v>0.569</v>
       </c>
       <c r="G5" t="n">
-        <v>0.707</v>
+        <v>0.571</v>
       </c>
       <c r="H5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.622</v>
+        <v>0.574</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.627</v>
       </c>
       <c r="F6" t="n">
-        <v>0.661</v>
+        <v>0.628</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.627</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -672,33 +672,33 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.632</v>
+        <v>0.582</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.637</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.626</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.637</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,33 +707,33 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.548</v>
+        <v>0.587</v>
       </c>
       <c r="E8" t="n">
-        <v>0.587</v>
+        <v>0.633</v>
       </c>
       <c r="F8" t="n">
-        <v>0.582</v>
+        <v>0.622</v>
       </c>
       <c r="G8" t="n">
-        <v>0.587</v>
+        <v>0.633</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I8" t="n">
-        <v>0.587</v>
+        <v>0.603</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -742,33 +742,33 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.601</v>
+        <v>0.414</v>
       </c>
       <c r="E9" t="n">
-        <v>0.667</v>
+        <v>0.472</v>
       </c>
       <c r="F9" t="n">
-        <v>0.636</v>
+        <v>0.46</v>
       </c>
       <c r="G9" t="n">
-        <v>0.667</v>
+        <v>0.472</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.667</v>
+        <v>0.468</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -777,28 +777,28 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.6</v>
+        <v>0.531</v>
       </c>
       <c r="E10" t="n">
-        <v>0.65</v>
+        <v>0.603</v>
       </c>
       <c r="F10" t="n">
-        <v>0.642</v>
+        <v>0.588</v>
       </c>
       <c r="G10" t="n">
-        <v>0.65</v>
+        <v>0.603</v>
       </c>
       <c r="H10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.635</v>
+        <v>0.603</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -812,33 +812,33 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.454</v>
+        <v>0.486</v>
       </c>
       <c r="E11" t="n">
-        <v>0.52</v>
+        <v>0.524</v>
       </c>
       <c r="F11" t="n">
-        <v>0.507</v>
+        <v>0.529</v>
       </c>
       <c r="G11" t="n">
-        <v>0.52</v>
+        <v>0.524</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.516</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -847,33 +847,33 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.647</v>
+        <v>0.597</v>
       </c>
       <c r="E12" t="n">
-        <v>0.694</v>
+        <v>0.659</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="G12" t="n">
-        <v>0.694</v>
+        <v>0.659</v>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -882,28 +882,28 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.486</v>
+        <v>0.524</v>
       </c>
       <c r="E13" t="n">
-        <v>0.524</v>
+        <v>0.548</v>
       </c>
       <c r="F13" t="n">
-        <v>0.529</v>
+        <v>0.553</v>
       </c>
       <c r="G13" t="n">
-        <v>0.524</v>
+        <v>0.548</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.524</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -917,33 +917,33 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.597</v>
+        <v>0.607</v>
       </c>
       <c r="E14" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.659</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.632</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.659</v>
-      </c>
-      <c r="H14" t="n">
-        <v>3</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.643</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -952,33 +952,33 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.582</v>
+        <v>0.626</v>
       </c>
       <c r="E15" t="n">
-        <v>0.637</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>0.626</v>
+        <v>0.663</v>
       </c>
       <c r="G15" t="n">
-        <v>0.637</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" t="n">
-        <v>0.627</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -987,22 +987,22 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.571</v>
       </c>
       <c r="E16" t="n">
-        <v>0.726</v>
+        <v>0.619</v>
       </c>
       <c r="F16" t="n">
-        <v>0.722</v>
+        <v>0.613</v>
       </c>
       <c r="G16" t="n">
-        <v>0.726</v>
+        <v>0.619</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.714</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="17">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1022,28 +1022,28 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.598</v>
+        <v>0.601</v>
       </c>
       <c r="E17" t="n">
-        <v>0.659</v>
+        <v>0.667</v>
       </c>
       <c r="F17" t="n">
-        <v>0.64</v>
+        <v>0.636</v>
       </c>
       <c r="G17" t="n">
-        <v>0.659</v>
+        <v>0.667</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.659</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1057,33 +1057,33 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.587</v>
+        <v>0.597</v>
       </c>
       <c r="E18" t="n">
-        <v>0.633</v>
+        <v>0.643</v>
       </c>
       <c r="F18" t="n">
-        <v>0.622</v>
+        <v>0.637</v>
       </c>
       <c r="G18" t="n">
-        <v>0.633</v>
+        <v>0.643</v>
       </c>
       <c r="H18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0.603</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1092,33 +1092,33 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.652</v>
+        <v>0.57</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.635</v>
       </c>
       <c r="F19" t="n">
-        <v>0.681</v>
+        <v>0.623</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.635</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1127,28 +1127,28 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.608</v>
+        <v>0.652</v>
       </c>
       <c r="E20" t="n">
-        <v>0.667</v>
+        <v>0.707</v>
       </c>
       <c r="F20" t="n">
-        <v>0.643</v>
+        <v>0.699</v>
       </c>
       <c r="G20" t="n">
-        <v>0.667</v>
+        <v>0.707</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I20" t="n">
-        <v>0.667</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1162,33 +1162,33 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.582</v>
+        <v>0.608</v>
       </c>
       <c r="E21" t="n">
-        <v>0.639</v>
+        <v>0.659</v>
       </c>
       <c r="F21" t="n">
-        <v>0.621</v>
+        <v>0.645</v>
       </c>
       <c r="G21" t="n">
-        <v>0.639</v>
+        <v>0.659</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0.619</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1197,33 +1197,33 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.654</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>0.696</v>
+        <v>0.603</v>
       </c>
       <c r="F22" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.595</v>
       </c>
       <c r="G22" t="n">
-        <v>0.696</v>
+        <v>0.603</v>
       </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.603</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1232,33 +1232,33 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.639</v>
+        <v>0.536</v>
       </c>
       <c r="E23" t="n">
-        <v>0.68</v>
+        <v>0.576</v>
       </c>
       <c r="F23" t="n">
-        <v>0.67</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="G23" t="n">
-        <v>0.68</v>
+        <v>0.576</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>0.675</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1267,33 +1267,33 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.594</v>
+        <v>0.647</v>
       </c>
       <c r="E24" t="n">
-        <v>0.656</v>
+        <v>0.694</v>
       </c>
       <c r="F24" t="n">
-        <v>0.631</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="G24" t="n">
-        <v>0.656</v>
+        <v>0.694</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" t="n">
-        <v>0.651</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1302,33 +1302,33 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.57</v>
+        <v>0.608</v>
       </c>
       <c r="E25" t="n">
-        <v>0.635</v>
+        <v>0.667</v>
       </c>
       <c r="F25" t="n">
-        <v>0.623</v>
+        <v>0.643</v>
       </c>
       <c r="G25" t="n">
-        <v>0.635</v>
+        <v>0.667</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.635</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1337,28 +1337,28 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.597</v>
+        <v>0.524</v>
       </c>
       <c r="E26" t="n">
-        <v>0.643</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="F26" t="n">
-        <v>0.637</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="G26" t="n">
-        <v>0.643</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>0.643</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.536</v>
+        <v>0.481</v>
       </c>
       <c r="E27" t="n">
-        <v>0.571</v>
+        <v>0.524</v>
       </c>
       <c r="F27" t="n">
-        <v>0.554</v>
+        <v>0.529</v>
       </c>
       <c r="G27" t="n">
-        <v>0.571</v>
+        <v>0.524</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>0.571</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="28">
@@ -1428,12 +1428,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1442,33 +1442,33 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.508</v>
+        <v>0.607</v>
       </c>
       <c r="E29" t="n">
-        <v>0.532</v>
+        <v>0.656</v>
       </c>
       <c r="F29" t="n">
-        <v>0.538</v>
+        <v>0.627</v>
       </c>
       <c r="G29" t="n">
-        <v>0.532</v>
+        <v>0.656</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="n">
-        <v>0.532</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1477,33 +1477,33 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.571</v>
+        <v>0.496</v>
       </c>
       <c r="E30" t="n">
-        <v>0.619</v>
+        <v>0.524</v>
       </c>
       <c r="F30" t="n">
-        <v>0.613</v>
+        <v>0.535</v>
       </c>
       <c r="G30" t="n">
-        <v>0.619</v>
+        <v>0.524</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0.619</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1512,33 +1512,33 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.668</v>
+        <v>0.605</v>
       </c>
       <c r="E31" t="n">
-        <v>0.717</v>
+        <v>0.656</v>
       </c>
       <c r="F31" t="n">
-        <v>0.714</v>
+        <v>0.643</v>
       </c>
       <c r="G31" t="n">
-        <v>0.717</v>
+        <v>0.656</v>
       </c>
       <c r="H31" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1547,33 +1547,33 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.51</v>
+        <v>0.338</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.333</v>
       </c>
       <c r="F32" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.275</v>
       </c>
       <c r="G32" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.333</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1582,28 +1582,28 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.614</v>
+        <v>0.596</v>
       </c>
       <c r="E33" t="n">
-        <v>0.675</v>
+        <v>0.656</v>
       </c>
       <c r="F33" t="n">
-        <v>0.664</v>
+        <v>0.652</v>
       </c>
       <c r="G33" t="n">
-        <v>0.675</v>
+        <v>0.656</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>0.675</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1617,28 +1617,28 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.509</v>
+        <v>0.508</v>
       </c>
       <c r="E34" t="n">
-        <v>0.571</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F34" t="n">
+        <v>0.555</v>
+      </c>
+      <c r="G34" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c r="G34" t="n">
-        <v>0.571</v>
-      </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>0.571</v>
+        <v>0.556</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1652,33 +1652,33 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.508</v>
+        <v>0.454</v>
       </c>
       <c r="E35" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="F35" t="n">
-        <v>0.555</v>
+        <v>0.507</v>
       </c>
       <c r="G35" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="H35" t="n">
         <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0.556</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1687,28 +1687,28 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.506</v>
+        <v>0.619</v>
       </c>
       <c r="E36" t="n">
-        <v>0.552</v>
+        <v>0.675</v>
       </c>
       <c r="F36" t="n">
-        <v>0.55</v>
+        <v>0.662</v>
       </c>
       <c r="G36" t="n">
-        <v>0.552</v>
+        <v>0.675</v>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.548</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1722,22 +1722,22 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.497</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="E37" t="n">
-        <v>0.516</v>
+        <v>0.726</v>
       </c>
       <c r="F37" t="n">
-        <v>0.522</v>
+        <v>0.722</v>
       </c>
       <c r="G37" t="n">
-        <v>0.516</v>
+        <v>0.726</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I37" t="n">
-        <v>0.516</v>
+        <v>0.714</v>
       </c>
     </row>
     <row r="38">
@@ -1778,12 +1778,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1792,33 +1792,33 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.531</v>
+        <v>0.497</v>
       </c>
       <c r="E39" t="n">
-        <v>0.603</v>
+        <v>0.516</v>
       </c>
       <c r="F39" t="n">
-        <v>0.588</v>
+        <v>0.522</v>
       </c>
       <c r="G39" t="n">
-        <v>0.603</v>
+        <v>0.516</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0.603</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1827,28 +1827,28 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.615</v>
+        <v>0.654</v>
       </c>
       <c r="E40" t="n">
-        <v>0.651</v>
+        <v>0.696</v>
       </c>
       <c r="F40" t="n">
-        <v>0.647</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="G40" t="n">
-        <v>0.651</v>
+        <v>0.696</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>0.651</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1862,33 +1862,33 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.648</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="E41" t="n">
-        <v>0.694</v>
+        <v>0.724</v>
       </c>
       <c r="F41" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="G41" t="n">
-        <v>0.694</v>
+        <v>0.724</v>
       </c>
       <c r="H41" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I41" t="n">
-        <v>0.667</v>
+        <v>0.706</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1897,33 +1897,33 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.548</v>
+        <v>0.59</v>
       </c>
       <c r="E42" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
       </c>
       <c r="F42" t="n">
-        <v>0.586</v>
+        <v>0.648</v>
       </c>
       <c r="G42" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1932,33 +1932,33 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.608</v>
+        <v>0.506</v>
       </c>
       <c r="E43" t="n">
-        <v>0.659</v>
+        <v>0.552</v>
       </c>
       <c r="F43" t="n">
-        <v>0.645</v>
+        <v>0.55</v>
       </c>
       <c r="G43" t="n">
-        <v>0.659</v>
+        <v>0.552</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="n">
-        <v>0.659</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1967,33 +1967,33 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.496</v>
+        <v>0.549</v>
       </c>
       <c r="E44" t="n">
-        <v>0.524</v>
+        <v>0.595</v>
       </c>
       <c r="F44" t="n">
-        <v>0.535</v>
+        <v>0.587</v>
       </c>
       <c r="G44" t="n">
-        <v>0.524</v>
+        <v>0.595</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>0.524</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2002,28 +2002,28 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.607</v>
+        <v>0.435</v>
       </c>
       <c r="E45" t="n">
-        <v>0.664</v>
+        <v>0.484</v>
       </c>
       <c r="F45" t="n">
-        <v>0.644</v>
+        <v>0.491</v>
       </c>
       <c r="G45" t="n">
-        <v>0.664</v>
+        <v>0.484</v>
       </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>0.659</v>
+        <v>0.484</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2037,33 +2037,33 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.516</v>
+        <v>0.645</v>
       </c>
       <c r="E46" t="n">
-        <v>0.571</v>
+        <v>0.68</v>
       </c>
       <c r="F46" t="n">
-        <v>0.569</v>
+        <v>0.67</v>
       </c>
       <c r="G46" t="n">
-        <v>0.571</v>
+        <v>0.68</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="n">
-        <v>0.571</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2072,33 +2072,33 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.524</v>
+        <v>0.597</v>
       </c>
       <c r="E47" t="n">
-        <v>0.548</v>
+        <v>0.659</v>
       </c>
       <c r="F47" t="n">
-        <v>0.553</v>
+        <v>0.632</v>
       </c>
       <c r="G47" t="n">
-        <v>0.548</v>
+        <v>0.659</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I47" t="n">
-        <v>0.548</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2107,28 +2107,28 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.611</v>
+        <v>0.508</v>
       </c>
       <c r="E48" t="n">
-        <v>0.675</v>
+        <v>0.532</v>
       </c>
       <c r="F48" t="n">
-        <v>0.647</v>
+        <v>0.538</v>
       </c>
       <c r="G48" t="n">
-        <v>0.675</v>
+        <v>0.532</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>0.675</v>
+        <v>0.532</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2142,33 +2142,33 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.619</v>
+        <v>0.617</v>
       </c>
       <c r="E49" t="n">
-        <v>0.675</v>
+        <v>0.664</v>
       </c>
       <c r="F49" t="n">
-        <v>0.662</v>
+        <v>0.651</v>
       </c>
       <c r="G49" t="n">
-        <v>0.675</v>
+        <v>0.664</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>0.675</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2177,33 +2177,33 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.596</v>
+        <v>0.317</v>
       </c>
       <c r="E50" t="n">
-        <v>0.656</v>
+        <v>0.385</v>
       </c>
       <c r="F50" t="n">
-        <v>0.652</v>
+        <v>0.295</v>
       </c>
       <c r="G50" t="n">
-        <v>0.656</v>
+        <v>0.385</v>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I50" t="n">
-        <v>0.651</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2212,28 +2212,28 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.605</v>
+        <v>0.648</v>
       </c>
       <c r="E51" t="n">
-        <v>0.656</v>
+        <v>0.694</v>
       </c>
       <c r="F51" t="n">
-        <v>0.643</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G51" t="n">
-        <v>0.656</v>
+        <v>0.694</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I51" t="n">
-        <v>0.651</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2247,33 +2247,33 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.338</v>
+        <v>0.638</v>
       </c>
       <c r="E52" t="n">
-        <v>0.333</v>
+        <v>0.675</v>
       </c>
       <c r="F52" t="n">
-        <v>0.275</v>
+        <v>0.669</v>
       </c>
       <c r="G52" t="n">
-        <v>0.333</v>
+        <v>0.675</v>
       </c>
       <c r="H52" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>0.063</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2282,33 +2282,33 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.341</v>
+        <v>0.587</v>
       </c>
       <c r="E53" t="n">
-        <v>0.413</v>
+        <v>0.643</v>
       </c>
       <c r="F53" t="n">
-        <v>0.401</v>
+        <v>0.626</v>
       </c>
       <c r="G53" t="n">
-        <v>0.413</v>
+        <v>0.643</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>0.413</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2317,22 +2317,22 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.549</v>
+        <v>0.548</v>
       </c>
       <c r="E54" t="n">
-        <v>0.595</v>
+        <v>0.587</v>
       </c>
       <c r="F54" t="n">
+        <v>0.582</v>
+      </c>
+      <c r="G54" t="n">
         <v>0.587</v>
       </c>
-      <c r="G54" t="n">
-        <v>0.595</v>
-      </c>
       <c r="H54" t="n">
         <v>0</v>
       </c>
       <c r="I54" t="n">
-        <v>0.595</v>
+        <v>0.587</v>
       </c>
     </row>
     <row r="55">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2352,22 +2352,22 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.481</v>
+        <v>0.614</v>
       </c>
       <c r="E55" t="n">
-        <v>0.524</v>
+        <v>0.664</v>
       </c>
       <c r="F55" t="n">
-        <v>0.529</v>
+        <v>0.648</v>
       </c>
       <c r="G55" t="n">
-        <v>0.524</v>
+        <v>0.664</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>0.524</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="56">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2387,33 +2387,33 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.622</v>
       </c>
       <c r="E56" t="n">
-        <v>0.724</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F56" t="n">
-        <v>0.72</v>
+        <v>0.661</v>
       </c>
       <c r="G56" t="n">
-        <v>0.724</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H56" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>0.706</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2422,33 +2422,33 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.607</v>
+        <v>0.536</v>
       </c>
       <c r="E57" t="n">
-        <v>0.656</v>
+        <v>0.571</v>
       </c>
       <c r="F57" t="n">
-        <v>0.627</v>
+        <v>0.554</v>
       </c>
       <c r="G57" t="n">
-        <v>0.656</v>
+        <v>0.571</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>0.651</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2457,28 +2457,28 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.574</v>
+        <v>0.615</v>
       </c>
       <c r="E58" t="n">
-        <v>0.627</v>
+        <v>0.651</v>
       </c>
       <c r="F58" t="n">
-        <v>0.628</v>
+        <v>0.647</v>
       </c>
       <c r="G58" t="n">
-        <v>0.627</v>
+        <v>0.651</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>0.627</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2492,19 +2492,19 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.645</v>
+        <v>0.611</v>
       </c>
       <c r="E59" t="n">
-        <v>0.68</v>
+        <v>0.675</v>
       </c>
       <c r="F59" t="n">
-        <v>0.67</v>
+        <v>0.647</v>
       </c>
       <c r="G59" t="n">
-        <v>0.68</v>
+        <v>0.675</v>
       </c>
       <c r="H59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>0.675</v>
@@ -2513,12 +2513,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2527,28 +2527,28 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.317</v>
+        <v>0.614</v>
       </c>
       <c r="E60" t="n">
-        <v>0.385</v>
+        <v>0.675</v>
       </c>
       <c r="F60" t="n">
-        <v>0.295</v>
+        <v>0.664</v>
       </c>
       <c r="G60" t="n">
-        <v>0.385</v>
+        <v>0.675</v>
       </c>
       <c r="H60" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>0.079</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2562,33 +2562,33 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.609</v>
+        <v>0.594</v>
       </c>
       <c r="E61" t="n">
-        <v>0.669</v>
+        <v>0.656</v>
       </c>
       <c r="F61" t="n">
-        <v>0.644</v>
+        <v>0.631</v>
       </c>
       <c r="G61" t="n">
-        <v>0.669</v>
+        <v>0.656</v>
       </c>
       <c r="H61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" t="n">
-        <v>0.659</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2597,19 +2597,19 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.617</v>
+        <v>0.598</v>
       </c>
       <c r="E62" t="n">
-        <v>0.664</v>
+        <v>0.659</v>
       </c>
       <c r="F62" t="n">
-        <v>0.651</v>
+        <v>0.64</v>
       </c>
       <c r="G62" t="n">
-        <v>0.664</v>
+        <v>0.659</v>
       </c>
       <c r="H62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" t="n">
         <v>0.659</v>
@@ -2618,12 +2618,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2632,28 +2632,28 @@
         </is>
       </c>
       <c r="D63" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="F63" t="n">
         <v>0.644</v>
       </c>
-      <c r="E63" t="n">
-        <v>0.698</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0.6909999999999999</v>
-      </c>
       <c r="G63" t="n">
-        <v>0.698</v>
+        <v>0.669</v>
       </c>
       <c r="H63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I63" t="n">
-        <v>0.698</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2667,33 +2667,33 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.597</v>
+        <v>0.509</v>
       </c>
       <c r="E64" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
       </c>
       <c r="F64" t="n">
-        <v>0.64</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G64" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2702,33 +2702,33 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.626</v>
+        <v>0.341</v>
       </c>
       <c r="E65" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.413</v>
       </c>
       <c r="F65" t="n">
-        <v>0.663</v>
+        <v>0.401</v>
       </c>
       <c r="G65" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.413</v>
       </c>
       <c r="H65" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>0.667</v>
+        <v>0.413</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2737,33 +2737,33 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.524</v>
+        <v>0.477</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="F66" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.496</v>
       </c>
       <c r="G66" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2772,33 +2772,33 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.638</v>
+        <v>0.668</v>
       </c>
       <c r="E67" t="n">
-        <v>0.675</v>
+        <v>0.717</v>
       </c>
       <c r="F67" t="n">
-        <v>0.669</v>
+        <v>0.714</v>
       </c>
       <c r="G67" t="n">
-        <v>0.675</v>
+        <v>0.717</v>
       </c>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I67" t="n">
-        <v>0.675</v>
+        <v>0.6830000000000001</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2807,28 +2807,28 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.414</v>
+        <v>0.639</v>
       </c>
       <c r="E68" t="n">
-        <v>0.472</v>
+        <v>0.68</v>
       </c>
       <c r="F68" t="n">
-        <v>0.46</v>
+        <v>0.67</v>
       </c>
       <c r="G68" t="n">
-        <v>0.472</v>
+        <v>0.68</v>
       </c>
       <c r="H68" t="n">
         <v>1</v>
       </c>
       <c r="I68" t="n">
-        <v>0.468</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2842,33 +2842,33 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.614</v>
+        <v>0.632</v>
       </c>
       <c r="E69" t="n">
-        <v>0.664</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F69" t="n">
-        <v>0.648</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G69" t="n">
-        <v>0.664</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
-        <v>0.659</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN12</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2877,33 +2877,33 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.536</v>
+        <v>0.51</v>
       </c>
       <c r="E70" t="n">
-        <v>0.576</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="F70" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="G70" t="n">
-        <v>0.576</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="H70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="n">
-        <v>0.571</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2912,28 +2912,28 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.621</v>
+        <v>0.548</v>
       </c>
       <c r="E71" t="n">
-        <v>0.667</v>
+        <v>0.595</v>
       </c>
       <c r="F71" t="n">
-        <v>0.659</v>
+        <v>0.586</v>
       </c>
       <c r="G71" t="n">
-        <v>0.667</v>
+        <v>0.595</v>
       </c>
       <c r="H71" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>0.651</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2947,33 +2947,33 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.587</v>
+        <v>0.621</v>
       </c>
       <c r="E72" t="n">
-        <v>0.643</v>
+        <v>0.667</v>
       </c>
       <c r="F72" t="n">
-        <v>0.626</v>
+        <v>0.659</v>
       </c>
       <c r="G72" t="n">
-        <v>0.643</v>
+        <v>0.667</v>
       </c>
       <c r="H72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I72" t="n">
-        <v>0.643</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2982,22 +2982,22 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.59</v>
+        <v>0.582</v>
       </c>
       <c r="E73" t="n">
-        <v>0.651</v>
+        <v>0.639</v>
       </c>
       <c r="F73" t="n">
-        <v>0.648</v>
+        <v>0.621</v>
       </c>
       <c r="G73" t="n">
-        <v>0.651</v>
+        <v>0.639</v>
       </c>
       <c r="H73" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I73" t="n">
-        <v>0.651</v>
+        <v>0.619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add avg F1 calculation and run experiments on fine-tuned Gemini-1.5-flash-001 (prompts N01-N10)
</commit_message>
<xml_diff>
--- a/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
+++ b/results/stage1_eval_initial_DR_prompts_126instances/summary_report/level1_metrics_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,16 @@
           <t>adjusted_accuracy</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>numeric_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -497,33 +502,36 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6</v>
+        <v>0.615</v>
       </c>
       <c r="E2" t="n">
-        <v>0.65</v>
+        <v>0.651</v>
       </c>
       <c r="F2" t="n">
-        <v>0.642</v>
+        <v>0.647</v>
       </c>
       <c r="G2" t="n">
-        <v>0.65</v>
+        <v>0.651</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.635</v>
+        <v>0.651</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,33 +540,36 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.644</v>
+        <v>0.497</v>
       </c>
       <c r="E3" t="n">
-        <v>0.698</v>
+        <v>0.516</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="G3" t="n">
-        <v>0.698</v>
+        <v>0.516</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.698</v>
+        <v>0.516</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -567,33 +578,36 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.652</v>
+        <v>0.638</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.675</v>
       </c>
       <c r="F4" t="n">
-        <v>0.681</v>
+        <v>0.669</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.675</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.675</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -602,33 +616,36 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.516</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>0.571</v>
+        <v>0.603</v>
       </c>
       <c r="F5" t="n">
-        <v>0.569</v>
+        <v>0.595</v>
       </c>
       <c r="G5" t="n">
-        <v>0.571</v>
+        <v>0.603</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.571</v>
+        <v>0.603</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-2.0-flash-exp</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -637,33 +654,36 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.574</v>
+        <v>0.573</v>
       </c>
       <c r="E6" t="n">
-        <v>0.627</v>
+        <v>0.659</v>
       </c>
       <c r="F6" t="n">
-        <v>0.628</v>
+        <v>0.647</v>
       </c>
       <c r="G6" t="n">
-        <v>0.627</v>
+        <v>0.659</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.627</v>
+        <v>0.659</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -672,33 +692,36 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.582</v>
+        <v>0.59</v>
       </c>
       <c r="E7" t="n">
-        <v>0.637</v>
+        <v>0.651</v>
       </c>
       <c r="F7" t="n">
-        <v>0.626</v>
+        <v>0.648</v>
       </c>
       <c r="G7" t="n">
-        <v>0.637</v>
+        <v>0.651</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.627</v>
+        <v>0.651</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,33 +730,36 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.587</v>
+        <v>0.596</v>
       </c>
       <c r="E8" t="n">
-        <v>0.633</v>
+        <v>0.656</v>
       </c>
       <c r="F8" t="n">
-        <v>0.622</v>
+        <v>0.652</v>
       </c>
       <c r="G8" t="n">
-        <v>0.633</v>
+        <v>0.656</v>
       </c>
       <c r="H8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.603</v>
+        <v>0.651</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN01</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -742,33 +768,36 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.414</v>
+        <v>0.597</v>
       </c>
       <c r="E9" t="n">
-        <v>0.472</v>
+        <v>0.643</v>
       </c>
       <c r="F9" t="n">
-        <v>0.46</v>
+        <v>0.637</v>
       </c>
       <c r="G9" t="n">
-        <v>0.472</v>
+        <v>0.643</v>
       </c>
       <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="J9" t="n">
         <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.468</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -777,33 +806,36 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.531</v>
+        <v>0.605</v>
       </c>
       <c r="E10" t="n">
-        <v>0.603</v>
+        <v>0.656</v>
       </c>
       <c r="F10" t="n">
-        <v>0.588</v>
+        <v>0.643</v>
       </c>
       <c r="G10" t="n">
-        <v>0.603</v>
+        <v>0.656</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.603</v>
+        <v>0.651</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -812,33 +844,36 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.486</v>
+        <v>0.608</v>
       </c>
       <c r="E11" t="n">
-        <v>0.524</v>
+        <v>0.635</v>
       </c>
       <c r="F11" t="n">
-        <v>0.529</v>
+        <v>0.637</v>
       </c>
       <c r="G11" t="n">
-        <v>0.524</v>
+        <v>0.635</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.524</v>
+        <v>0.635</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -847,33 +882,36 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.597</v>
+        <v>0.632</v>
       </c>
       <c r="E12" t="n">
-        <v>0.659</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>0.64</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G12" t="n">
-        <v>0.659</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.659</v>
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -882,33 +920,36 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.524</v>
+        <v>0.574</v>
       </c>
       <c r="E13" t="n">
-        <v>0.548</v>
+        <v>0.627</v>
       </c>
       <c r="F13" t="n">
-        <v>0.553</v>
+        <v>0.628</v>
       </c>
       <c r="G13" t="n">
-        <v>0.548</v>
+        <v>0.627</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.548</v>
+        <v>0.627</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -917,28 +958,31 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.607</v>
+        <v>0.548</v>
       </c>
       <c r="E14" t="n">
-        <v>0.664</v>
+        <v>0.595</v>
       </c>
       <c r="F14" t="n">
-        <v>0.644</v>
+        <v>0.586</v>
       </c>
       <c r="G14" t="n">
-        <v>0.664</v>
+        <v>0.595</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.659</v>
+        <v>0.595</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -952,33 +996,36 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.626</v>
+        <v>0.617</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.664</v>
       </c>
       <c r="F15" t="n">
-        <v>0.663</v>
+        <v>0.651</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.664</v>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.667</v>
+        <v>0.659</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN02</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -987,33 +1034,36 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.571</v>
+        <v>0.644</v>
       </c>
       <c r="E16" t="n">
-        <v>0.619</v>
+        <v>0.698</v>
       </c>
       <c r="F16" t="n">
-        <v>0.613</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="G16" t="n">
-        <v>0.619</v>
+        <v>0.698</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.619</v>
+        <v>0.698</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1022,33 +1072,36 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.601</v>
+        <v>0.53</v>
       </c>
       <c r="E17" t="n">
-        <v>0.667</v>
+        <v>0.556</v>
       </c>
       <c r="F17" t="n">
-        <v>0.636</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>0.667</v>
+        <v>0.556</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.667</v>
+        <v>0.556</v>
+      </c>
+      <c r="J17" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1057,28 +1110,31 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.597</v>
+        <v>0.594</v>
       </c>
       <c r="E18" t="n">
-        <v>0.643</v>
+        <v>0.656</v>
       </c>
       <c r="F18" t="n">
-        <v>0.637</v>
+        <v>0.631</v>
       </c>
       <c r="G18" t="n">
-        <v>0.643</v>
+        <v>0.656</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>0.643</v>
+        <v>0.651</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1092,33 +1148,36 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.57</v>
+        <v>0.587</v>
       </c>
       <c r="E19" t="n">
-        <v>0.635</v>
+        <v>0.643</v>
       </c>
       <c r="F19" t="n">
-        <v>0.623</v>
+        <v>0.626</v>
       </c>
       <c r="G19" t="n">
-        <v>0.635</v>
+        <v>0.643</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.635</v>
+        <v>0.643</v>
+      </c>
+      <c r="J19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1127,22 +1186,25 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.652</v>
+        <v>0.607</v>
       </c>
       <c r="E20" t="n">
-        <v>0.707</v>
+        <v>0.664</v>
       </c>
       <c r="F20" t="n">
-        <v>0.699</v>
+        <v>0.644</v>
       </c>
       <c r="G20" t="n">
-        <v>0.707</v>
+        <v>0.664</v>
       </c>
       <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="J20" t="n">
         <v>3</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1153,7 +1215,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1162,28 +1224,31 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.608</v>
+        <v>0.536</v>
       </c>
       <c r="E21" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
       </c>
       <c r="F21" t="n">
-        <v>0.645</v>
+        <v>0.554</v>
       </c>
       <c r="G21" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0.659</v>
+        <v>0.571</v>
+      </c>
+      <c r="J21" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1197,33 +1262,36 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.571</v>
       </c>
       <c r="E22" t="n">
-        <v>0.603</v>
+        <v>0.619</v>
       </c>
       <c r="F22" t="n">
-        <v>0.595</v>
+        <v>0.613</v>
       </c>
       <c r="G22" t="n">
-        <v>0.603</v>
+        <v>0.619</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>0.603</v>
+        <v>0.619</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1232,33 +1300,36 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.536</v>
+        <v>0.608</v>
       </c>
       <c r="E23" t="n">
-        <v>0.576</v>
+        <v>0.659</v>
       </c>
       <c r="F23" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.645</v>
       </c>
       <c r="G23" t="n">
-        <v>0.576</v>
+        <v>0.659</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.571</v>
+        <v>0.659</v>
+      </c>
+      <c r="J23" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1267,33 +1338,36 @@
         </is>
       </c>
       <c r="D24" t="n">
+        <v>0.611</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="F24" t="n">
         <v>0.647</v>
       </c>
-      <c r="E24" t="n">
-        <v>0.694</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.6860000000000001</v>
-      </c>
       <c r="G24" t="n">
-        <v>0.694</v>
+        <v>0.675</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.675</v>
+      </c>
+      <c r="J24" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1302,33 +1376,36 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.608</v>
+        <v>0.528</v>
       </c>
       <c r="E25" t="n">
-        <v>0.667</v>
+        <v>0.548</v>
       </c>
       <c r="F25" t="n">
-        <v>0.643</v>
+        <v>0.551</v>
       </c>
       <c r="G25" t="n">
-        <v>0.667</v>
+        <v>0.548</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.667</v>
+        <v>0.548</v>
+      </c>
+      <c r="J25" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1337,28 +1414,31 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.524</v>
+        <v>0.614</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.675</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.664</v>
       </c>
       <c r="G26" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.675</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.675</v>
+      </c>
+      <c r="J26" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1372,33 +1452,36 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.481</v>
+        <v>0.598</v>
       </c>
       <c r="E27" t="n">
-        <v>0.524</v>
+        <v>0.659</v>
       </c>
       <c r="F27" t="n">
-        <v>0.529</v>
+        <v>0.64</v>
       </c>
       <c r="G27" t="n">
-        <v>0.524</v>
+        <v>0.659</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>0.524</v>
+        <v>0.659</v>
+      </c>
+      <c r="J27" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1407,33 +1490,36 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.656</v>
+        <v>0.57</v>
       </c>
       <c r="E28" t="n">
-        <v>0.696</v>
+        <v>0.635</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.623</v>
       </c>
       <c r="G28" t="n">
-        <v>0.696</v>
+        <v>0.635</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.635</v>
+      </c>
+      <c r="J28" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1442,33 +1528,36 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.607</v>
+        <v>0.597</v>
       </c>
       <c r="E29" t="n">
-        <v>0.656</v>
+        <v>0.659</v>
       </c>
       <c r="F29" t="n">
-        <v>0.627</v>
+        <v>0.64</v>
       </c>
       <c r="G29" t="n">
-        <v>0.656</v>
+        <v>0.659</v>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>0.651</v>
+        <v>0.659</v>
+      </c>
+      <c r="J29" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN04</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1477,33 +1566,36 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.496</v>
+        <v>0.601</v>
       </c>
       <c r="E30" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
       </c>
       <c r="F30" t="n">
-        <v>0.535</v>
+        <v>0.636</v>
       </c>
       <c r="G30" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0.524</v>
+        <v>0.667</v>
+      </c>
+      <c r="J30" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1512,33 +1604,36 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.605</v>
+        <v>0.508</v>
       </c>
       <c r="E31" t="n">
-        <v>0.656</v>
+        <v>0.54</v>
       </c>
       <c r="F31" t="n">
-        <v>0.643</v>
+        <v>0.55</v>
       </c>
       <c r="G31" t="n">
-        <v>0.656</v>
+        <v>0.54</v>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>0.651</v>
+        <v>0.54</v>
+      </c>
+      <c r="J31" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1547,33 +1642,36 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.338</v>
+        <v>0.622</v>
       </c>
       <c r="E32" t="n">
-        <v>0.333</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F32" t="n">
-        <v>0.275</v>
+        <v>0.661</v>
       </c>
       <c r="G32" t="n">
-        <v>0.333</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H32" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>0.063</v>
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="J32" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1582,33 +1680,36 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.596</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="E33" t="n">
-        <v>0.656</v>
+        <v>0.724</v>
       </c>
       <c r="F33" t="n">
-        <v>0.652</v>
+        <v>0.72</v>
       </c>
       <c r="G33" t="n">
-        <v>0.656</v>
+        <v>0.724</v>
       </c>
       <c r="H33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33" t="n">
-        <v>0.651</v>
+        <v>0.706</v>
+      </c>
+      <c r="J33" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1617,28 +1718,31 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.508</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.726</v>
       </c>
       <c r="F34" t="n">
-        <v>0.555</v>
+        <v>0.722</v>
       </c>
       <c r="G34" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.726</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" t="n">
-        <v>0.556</v>
+        <v>0.714</v>
+      </c>
+      <c r="J34" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1652,33 +1756,36 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.454</v>
+        <v>0.509</v>
       </c>
       <c r="E35" t="n">
-        <v>0.52</v>
+        <v>0.571</v>
       </c>
       <c r="F35" t="n">
-        <v>0.507</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G35" t="n">
-        <v>0.52</v>
+        <v>0.571</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>0.516</v>
+        <v>0.571</v>
+      </c>
+      <c r="J35" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN05</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1687,22 +1794,25 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.619</v>
+        <v>0.531</v>
       </c>
       <c r="E36" t="n">
-        <v>0.675</v>
+        <v>0.603</v>
       </c>
       <c r="F36" t="n">
-        <v>0.662</v>
+        <v>0.588</v>
       </c>
       <c r="G36" t="n">
-        <v>0.675</v>
+        <v>0.603</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.675</v>
+        <v>0.603</v>
+      </c>
+      <c r="J36" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1713,7 +1823,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1722,28 +1832,31 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.608</v>
       </c>
       <c r="E37" t="n">
-        <v>0.726</v>
+        <v>0.667</v>
       </c>
       <c r="F37" t="n">
-        <v>0.722</v>
+        <v>0.643</v>
       </c>
       <c r="G37" t="n">
-        <v>0.726</v>
+        <v>0.667</v>
       </c>
       <c r="H37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0.714</v>
+        <v>0.667</v>
+      </c>
+      <c r="J37" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1757,33 +1870,36 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.471</v>
+        <v>0.435</v>
       </c>
       <c r="E38" t="n">
-        <v>0.532</v>
+        <v>0.484</v>
       </c>
       <c r="F38" t="n">
-        <v>0.502</v>
+        <v>0.491</v>
       </c>
       <c r="G38" t="n">
-        <v>0.532</v>
+        <v>0.484</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>0.532</v>
+        <v>0.484</v>
+      </c>
+      <c r="J38" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1792,22 +1908,25 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.497</v>
+        <v>0.597</v>
       </c>
       <c r="E39" t="n">
-        <v>0.516</v>
+        <v>0.635</v>
       </c>
       <c r="F39" t="n">
-        <v>0.522</v>
+        <v>0.64</v>
       </c>
       <c r="G39" t="n">
-        <v>0.516</v>
+        <v>0.635</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0.516</v>
+        <v>0.635</v>
+      </c>
+      <c r="J39" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -1827,33 +1946,36 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.654</v>
+        <v>0.619</v>
       </c>
       <c r="E40" t="n">
-        <v>0.696</v>
+        <v>0.675</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.662</v>
       </c>
       <c r="G40" t="n">
-        <v>0.696</v>
+        <v>0.675</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.675</v>
+      </c>
+      <c r="J40" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1862,33 +1984,36 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.481</v>
       </c>
       <c r="E41" t="n">
-        <v>0.724</v>
+        <v>0.524</v>
       </c>
       <c r="F41" t="n">
-        <v>0.72</v>
+        <v>0.529</v>
       </c>
       <c r="G41" t="n">
-        <v>0.724</v>
+        <v>0.524</v>
       </c>
       <c r="H41" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>0.706</v>
+        <v>0.524</v>
+      </c>
+      <c r="J41" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1897,33 +2022,36 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.59</v>
+        <v>0.614</v>
       </c>
       <c r="E42" t="n">
-        <v>0.651</v>
+        <v>0.664</v>
       </c>
       <c r="F42" t="n">
         <v>0.648</v>
       </c>
       <c r="G42" t="n">
-        <v>0.651</v>
+        <v>0.664</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>0.651</v>
+        <v>0.659</v>
+      </c>
+      <c r="J42" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1932,28 +2060,31 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.506</v>
+        <v>0.647</v>
       </c>
       <c r="E43" t="n">
-        <v>0.552</v>
+        <v>0.694</v>
       </c>
       <c r="F43" t="n">
-        <v>0.55</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="G43" t="n">
-        <v>0.552</v>
+        <v>0.694</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" t="n">
-        <v>0.548</v>
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="J43" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN06</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1967,33 +2098,36 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.549</v>
+        <v>0.654</v>
       </c>
       <c r="E44" t="n">
-        <v>0.595</v>
+        <v>0.696</v>
       </c>
       <c r="F44" t="n">
-        <v>0.587</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="G44" t="n">
-        <v>0.595</v>
+        <v>0.696</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="n">
-        <v>0.595</v>
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="J44" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2002,33 +2136,36 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.435</v>
+        <v>0.538</v>
       </c>
       <c r="E45" t="n">
-        <v>0.484</v>
+        <v>0.556</v>
       </c>
       <c r="F45" t="n">
-        <v>0.491</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="G45" t="n">
-        <v>0.484</v>
+        <v>0.556</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>0.484</v>
+        <v>0.556</v>
+      </c>
+      <c r="J45" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2037,33 +2174,36 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.645</v>
+        <v>0.582</v>
       </c>
       <c r="E46" t="n">
-        <v>0.68</v>
+        <v>0.637</v>
       </c>
       <c r="F46" t="n">
-        <v>0.67</v>
+        <v>0.626</v>
       </c>
       <c r="G46" t="n">
-        <v>0.68</v>
+        <v>0.637</v>
       </c>
       <c r="H46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" t="n">
-        <v>0.675</v>
+        <v>0.627</v>
+      </c>
+      <c r="J46" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2072,28 +2212,31 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.597</v>
+        <v>0.506</v>
       </c>
       <c r="E47" t="n">
-        <v>0.659</v>
+        <v>0.552</v>
       </c>
       <c r="F47" t="n">
-        <v>0.632</v>
+        <v>0.55</v>
       </c>
       <c r="G47" t="n">
-        <v>0.659</v>
+        <v>0.552</v>
       </c>
       <c r="H47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>0.643</v>
+        <v>0.548</v>
+      </c>
+      <c r="J47" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2107,28 +2250,31 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.508</v>
+        <v>0.621</v>
       </c>
       <c r="E48" t="n">
-        <v>0.532</v>
+        <v>0.667</v>
       </c>
       <c r="F48" t="n">
-        <v>0.538</v>
+        <v>0.659</v>
       </c>
       <c r="G48" t="n">
-        <v>0.532</v>
+        <v>0.667</v>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I48" t="n">
-        <v>0.532</v>
+        <v>0.651</v>
+      </c>
+      <c r="J48" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2142,28 +2288,31 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.617</v>
+        <v>0.652</v>
       </c>
       <c r="E49" t="n">
-        <v>0.664</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F49" t="n">
-        <v>0.651</v>
+        <v>0.681</v>
       </c>
       <c r="G49" t="n">
-        <v>0.664</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>0.659</v>
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="J49" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>promptN11</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2177,33 +2326,36 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.317</v>
+        <v>0.508</v>
       </c>
       <c r="E50" t="n">
-        <v>0.385</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F50" t="n">
-        <v>0.295</v>
+        <v>0.555</v>
       </c>
       <c r="G50" t="n">
-        <v>0.385</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H50" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>0.079</v>
+        <v>0.556</v>
+      </c>
+      <c r="J50" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>promptN08</t>
+          <t>promptN07</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2212,33 +2364,36 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.648</v>
+        <v>0.639</v>
       </c>
       <c r="E51" t="n">
-        <v>0.694</v>
+        <v>0.68</v>
       </c>
       <c r="F51" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="G51" t="n">
-        <v>0.694</v>
+        <v>0.68</v>
       </c>
       <c r="H51" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>0.667</v>
+        <v>0.675</v>
+      </c>
+      <c r="J51" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2247,33 +2402,36 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.638</v>
+        <v>0.648</v>
       </c>
       <c r="E52" t="n">
-        <v>0.675</v>
+        <v>0.694</v>
       </c>
       <c r="F52" t="n">
-        <v>0.669</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G52" t="n">
-        <v>0.675</v>
+        <v>0.694</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I52" t="n">
-        <v>0.675</v>
+        <v>0.667</v>
+      </c>
+      <c r="J52" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2282,33 +2440,36 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.587</v>
+        <v>0.533</v>
       </c>
       <c r="E53" t="n">
-        <v>0.643</v>
+        <v>0.571</v>
       </c>
       <c r="F53" t="n">
-        <v>0.626</v>
+        <v>0.574</v>
       </c>
       <c r="G53" t="n">
-        <v>0.643</v>
+        <v>0.571</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>0.643</v>
+        <v>0.571</v>
+      </c>
+      <c r="J53" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2317,28 +2478,31 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.548</v>
+        <v>0.656</v>
       </c>
       <c r="E54" t="n">
-        <v>0.587</v>
+        <v>0.696</v>
       </c>
       <c r="F54" t="n">
-        <v>0.582</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G54" t="n">
-        <v>0.587</v>
+        <v>0.696</v>
       </c>
       <c r="H54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" t="n">
-        <v>0.587</v>
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="J54" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>promptN06</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2352,33 +2516,36 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.614</v>
+        <v>0.652</v>
       </c>
       <c r="E55" t="n">
-        <v>0.664</v>
+        <v>0.707</v>
       </c>
       <c r="F55" t="n">
-        <v>0.648</v>
+        <v>0.699</v>
       </c>
       <c r="G55" t="n">
-        <v>0.664</v>
+        <v>0.707</v>
       </c>
       <c r="H55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I55" t="n">
-        <v>0.659</v>
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="J55" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2387,33 +2554,36 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.622</v>
+        <v>0.454</v>
       </c>
       <c r="E56" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="F56" t="n">
-        <v>0.661</v>
+        <v>0.507</v>
       </c>
       <c r="G56" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.516</v>
+      </c>
+      <c r="J56" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2422,33 +2592,36 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.536</v>
+        <v>0.645</v>
       </c>
       <c r="E57" t="n">
-        <v>0.571</v>
+        <v>0.68</v>
       </c>
       <c r="F57" t="n">
-        <v>0.554</v>
+        <v>0.67</v>
       </c>
       <c r="G57" t="n">
-        <v>0.571</v>
+        <v>0.68</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="n">
-        <v>0.571</v>
+        <v>0.675</v>
+      </c>
+      <c r="J57" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>promptN01</t>
+          <t>promptN08</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2457,28 +2630,31 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.615</v>
+        <v>0.471</v>
       </c>
       <c r="E58" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
       </c>
       <c r="F58" t="n">
-        <v>0.647</v>
+        <v>0.502</v>
       </c>
       <c r="G58" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>0.651</v>
+        <v>0.532</v>
+      </c>
+      <c r="J58" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2492,33 +2668,36 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.611</v>
+        <v>0.609</v>
       </c>
       <c r="E59" t="n">
-        <v>0.675</v>
+        <v>0.669</v>
       </c>
       <c r="F59" t="n">
-        <v>0.647</v>
+        <v>0.644</v>
       </c>
       <c r="G59" t="n">
-        <v>0.675</v>
+        <v>0.669</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I59" t="n">
-        <v>0.675</v>
+        <v>0.659</v>
+      </c>
+      <c r="J59" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2527,33 +2706,36 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.614</v>
+        <v>0.548</v>
       </c>
       <c r="E60" t="n">
-        <v>0.675</v>
+        <v>0.587</v>
       </c>
       <c r="F60" t="n">
-        <v>0.664</v>
+        <v>0.582</v>
       </c>
       <c r="G60" t="n">
-        <v>0.675</v>
+        <v>0.587</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>0.675</v>
+        <v>0.587</v>
+      </c>
+      <c r="J60" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>promptN03</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2562,33 +2744,36 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.594</v>
+        <v>0.668</v>
       </c>
       <c r="E61" t="n">
-        <v>0.656</v>
+        <v>0.717</v>
       </c>
       <c r="F61" t="n">
-        <v>0.631</v>
+        <v>0.714</v>
       </c>
       <c r="G61" t="n">
-        <v>0.656</v>
+        <v>0.717</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I61" t="n">
-        <v>0.651</v>
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="J61" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>promptN04</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2597,22 +2782,25 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.598</v>
+        <v>0.6</v>
       </c>
       <c r="E62" t="n">
-        <v>0.659</v>
+        <v>0.65</v>
       </c>
       <c r="F62" t="n">
-        <v>0.64</v>
+        <v>0.642</v>
       </c>
       <c r="G62" t="n">
-        <v>0.659</v>
+        <v>0.65</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I62" t="n">
-        <v>0.659</v>
+        <v>0.635</v>
+      </c>
+      <c r="J62" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="63">
@@ -2623,7 +2811,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2632,33 +2820,36 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.609</v>
+        <v>0.531</v>
       </c>
       <c r="E63" t="n">
-        <v>0.669</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="F63" t="n">
-        <v>0.644</v>
+        <v>0.571</v>
       </c>
       <c r="G63" t="n">
-        <v>0.669</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="H63" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
-        <v>0.659</v>
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="J63" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>promptN05</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2667,28 +2858,31 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.509</v>
+        <v>0.626</v>
       </c>
       <c r="E64" t="n">
-        <v>0.571</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F64" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.663</v>
       </c>
       <c r="G64" t="n">
-        <v>0.571</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I64" t="n">
-        <v>0.571</v>
+        <v>0.667</v>
+      </c>
+      <c r="J64" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN09</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2702,33 +2896,36 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.341</v>
+        <v>0.536</v>
       </c>
       <c r="E65" t="n">
-        <v>0.413</v>
+        <v>0.576</v>
       </c>
       <c r="F65" t="n">
-        <v>0.401</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="G65" t="n">
-        <v>0.413</v>
+        <v>0.576</v>
       </c>
       <c r="H65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" t="n">
-        <v>0.413</v>
+        <v>0.571</v>
+      </c>
+      <c r="J65" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2737,33 +2934,36 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.477</v>
+        <v>0.587</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5</v>
+        <v>0.633</v>
       </c>
       <c r="F66" t="n">
-        <v>0.496</v>
+        <v>0.622</v>
       </c>
       <c r="G66" t="n">
-        <v>0.5</v>
+        <v>0.633</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I66" t="n">
-        <v>0.5</v>
+        <v>0.603</v>
+      </c>
+      <c r="J66" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>promptN09</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2772,33 +2972,36 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.668</v>
+        <v>0.414</v>
       </c>
       <c r="E67" t="n">
-        <v>0.717</v>
+        <v>0.472</v>
       </c>
       <c r="F67" t="n">
-        <v>0.714</v>
+        <v>0.46</v>
       </c>
       <c r="G67" t="n">
-        <v>0.717</v>
+        <v>0.472</v>
       </c>
       <c r="H67" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I67" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.468</v>
+      </c>
+      <c r="J67" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2807,33 +3010,36 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.639</v>
+        <v>0.341</v>
       </c>
       <c r="E68" t="n">
-        <v>0.68</v>
+        <v>0.413</v>
       </c>
       <c r="F68" t="n">
-        <v>0.67</v>
+        <v>0.401</v>
       </c>
       <c r="G68" t="n">
-        <v>0.68</v>
+        <v>0.413</v>
       </c>
       <c r="H68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="n">
-        <v>0.675</v>
+        <v>0.413</v>
+      </c>
+      <c r="J68" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-flash-001-tuning</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2842,33 +3048,36 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.632</v>
+        <v>0.545</v>
       </c>
       <c r="E69" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.579</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.586</v>
       </c>
       <c r="G69" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.579</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
       </c>
       <c r="I69" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.579</v>
+      </c>
+      <c r="J69" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>promptN12</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2877,33 +3086,36 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.51</v>
+        <v>0.582</v>
       </c>
       <c r="E70" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.639</v>
       </c>
       <c r="F70" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.621</v>
       </c>
       <c r="G70" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.639</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I70" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.619</v>
+      </c>
+      <c r="J70" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>promptN02</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2912,33 +3124,36 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.548</v>
+        <v>0.607</v>
       </c>
       <c r="E71" t="n">
-        <v>0.595</v>
+        <v>0.656</v>
       </c>
       <c r="F71" t="n">
-        <v>0.586</v>
+        <v>0.627</v>
       </c>
       <c r="G71" t="n">
-        <v>0.595</v>
+        <v>0.656</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" t="n">
-        <v>0.595</v>
+        <v>0.651</v>
+      </c>
+      <c r="J71" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>promptN07</t>
+          <t>promptN10</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>claude-3-5-sonnet-20241022</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2947,57 +3162,481 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.621</v>
+        <v>0.597</v>
       </c>
       <c r="E72" t="n">
-        <v>0.667</v>
+        <v>0.659</v>
       </c>
       <c r="F72" t="n">
+        <v>0.632</v>
+      </c>
+      <c r="G72" t="n">
         <v>0.659</v>
-      </c>
-      <c r="G72" t="n">
-        <v>0.667</v>
       </c>
       <c r="H72" t="n">
         <v>3</v>
       </c>
       <c r="I72" t="n">
-        <v>0.651</v>
+        <v>0.643</v>
+      </c>
+      <c r="J72" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>promptN10</t>
+          <t>promptN11</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.317</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="H73" t="n">
+        <v>100</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="J73" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="H74" t="n">
+        <v>102</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="J74" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>claude-3-5-sonnet-20241022</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>level1</t>
-        </is>
-      </c>
-      <c r="D73" t="n">
-        <v>0.582</v>
-      </c>
-      <c r="E73" t="n">
-        <v>0.639</v>
-      </c>
-      <c r="F73" t="n">
-        <v>0.621</v>
-      </c>
-      <c r="G73" t="n">
-        <v>0.639</v>
-      </c>
-      <c r="H73" t="n">
-        <v>4</v>
-      </c>
-      <c r="I73" t="n">
-        <v>0.619</v>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.548</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.548</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.548</v>
+      </c>
+      <c r="J75" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="J76" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="J77" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>promptN11</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="J78" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.496</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="J79" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.496</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J80" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.529</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="J81" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.5610000000000001</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="J82" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="J83" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>promptN12</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>claude-3-5-sonnet-20241022</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>level1</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.508</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.532</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.532</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.532</v>
+      </c>
+      <c r="J84" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>